<commit_message>
Mise a jour logo
</commit_message>
<xml_diff>
--- a/src/assets/data/portraits_content.xlsx
+++ b/src/assets/data/portraits_content.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="391">
   <si>
     <t>id</t>
   </si>
@@ -774,6 +774,101 @@
   </si>
   <si>
     <t>M187.75,62.15c17.94-66.3-45-59.24-89.63-61.54C38-4.74,27.07,25.32,23.67,79.23c-5.11,32.15-46.86,77.28-5.72,100.4,13.57,7.64,29.52,7,44.68,6.12,26.72-4,80.56,2.74,99.19-14.46,17.83-18.24,10.91-48.27,14.88-71.51C178.91,86.79,184.32,74.8,187.75,62.15Z</t>
+  </si>
+  <si>
+    <t>strength_logo</t>
+  </si>
+  <si>
+    <t>M282.57,188c-11.74,7.05-18.12,16.18-25.65,27.32-1.49,2.2-3.13,4.42-5.44,5.75s-5.46,1.53-7.49-.19c-2.74-2.33-2.2-6.62-1.41-10.12,2.64-11.83,5.88-23.31,5.76-35.49a100.83,100.83,0,0,0-5.27-30.94c-6.61-19.68-19.21-37.47-36.3-49.38-32-22.29-77.71-22.69-110.09-1S47.35,158.2,55.87,196.26s41.94,69.24,80.49,75.11c9.29,1.41,19.16,1.6,27.23,6.4,16.07,9.55,17.58,32.71,11.73,50.46s-17,33.78-20,52.22c-4.6,28.15,13.21,58.31,40.07,67.88s59.73-2.51,74-27.22c7.55-13.08,8.83-27.81,6.35-42.39-2.33-13.64-8.76-23.1-18.38-33-9.07-9.3-19-19.2-22.08-32.28-.79-3.28-.55-6.95,1.4-9.7s5.87-4.2,8.89-2.7a12.06,12.06,0,0,1,4,3.92c10.29,14,21.81,27.09,38.65,33.37,39,16.48,83.78-.22,104.33-36.71a79.08,79.08,0,0,0,8.91-24.29c7.49-40.3-18.89-84.45-58.21-96.37a76.82,76.82,0,0,0-51.33,2.31A70.79,70.79,0,0,0,282.57,188Z</t>
+  </si>
+  <si>
+    <t>palmares_logo</t>
+  </si>
+  <si>
+    <t>M111.45,64.69a16.85,16.85,0,0,0-2.17,1.08,17.5,17.5,0,0,0-7.27,8c-1.16,2.83-.46,6.39-3.76,7.84-1.67.73-4.35-5-5.3-6a14.15,14.15,0,0,0-9.16-4.08c-6.05-.38-11.23,3.17-14.26,8.2-4.41,7.34-5.53,17.93-2.24,27.05,1.78,4.92,4.79,9.27,3.62,10.26-.66.55-6.74-1.37-7.76-1.56-3.23-.59-6.48-1.1-9.74-1.5a93.24,93.24,0,0,0-20.65-.55c-12.3,1.27-28.14,9.59-24.82,24.37,1.45,6.43,6.58,10.48,11.85,13.87,5.52,3.55,9.62,3.93,9.69,6,.09,2.72-7.3,3.33-14.76,8.32C7,171.16-1.46,181.56.21,190.38c1.46,7.69,9.66,11.66,16.47,13.54,15.6,4.3,32.34,1.47,46.8-5.31,6-2.79,11.92-6,16.71-10.59A24.24,24.24,0,0,0,86,180c1.39-3.3.84-6.79,2.88-9.8,9.4-2.54,19.94-2,26.11-11.28,4.49-7.34,7-14.22-.29-22.2-4.8-3.91-5.33-4.24-1.79-9.54,2-4,1.56-8.37,1.12-12.68-.46-4.6-1.55-6.81-.48-7.6,1.23-.92,6.41,1.47,8.19,1.39a19.21,19.21,0,0,0,10.44-3.66c8.36-6.13,10.92-19.62,6.37-28.73C133.74,66.31,121.62,60.44,111.45,64.69ZM62.16,170.56c7.1-.56,6.15,6.62,1.6,9.86-8.41,8.28-38.2,17.45-48.85,11.47-3.32-3.2.61-8.43,3.42-10.34,3-2.08,6.7-3,10.15-4.11C39.38,173.74,50.58,170.78,62.16,170.56Zm-3-37.42c6.74,1,51.67,9.32,46.9,18.39-5.39,10-53.75-3.5-63.18-7.63-4.79-1.48-16.53-5.42-10.11-11.73C37.36,128.7,52.87,132.74,59.17,133.14ZM92.9,101.36a39.53,39.53,0,0,1,7,15.14c1.33,9.06-7.37,5.09-10.22.33-5-6.83-10.87-15.68-11.34-24.25C80.4,86.38,91.18,98.81,92.9,101.36ZM122.06,81c13.29,7.29,5.78,13.38-5.31,8.38C107.58,84.74,114,76.55,122.06,81Z</t>
+  </si>
+  <si>
+    <t>city_logo</t>
+  </si>
+  <si>
+    <t>M195.41,399.11c51.69-89-71.48-160.19-131-77.51-22.31,26.62-5.06,65.6,31.22,55,18.19-5.71,23.94-27.17,38-38.54,12.93-8.29,22.08,10.27,13.78,20.27-7.29,12.22-20.7,20.5-25.68,33.84-8.29,20.8,10.57,44.58,32.72,41.18C172.88,430.32,185.52,413.7,195.41,399.11Z</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">Quel.le </t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>sportif.ve</t>
+    </r>
+    <r>
+      <rPr/>
+      <t xml:space="preserve"> es tu?</t>
+    </r>
+  </si>
+  <si>
+    <t>personalitly_logo</t>
+  </si>
+  <si>
+    <t>M293.9,151.74c-2.88-17.18-24.63-27.53-38.62-16-2.95,3-8.86,7.57-12.07,2.53-1.25-3,1.72-4.41,3.92-5.15,15.8-3.7,28-20.35,18.47-35.68-15.3-20.4-40.74-8.06-41.34,15.84-1.87,6.07-9.64,9.12-11.43,1.11C212,102.65,223.3,96.08,216,82.43c-7.06-14.37-27.38-18.15-40-8.85-17.6,12-14.12,41,5.82,48.44,3.53,1.42,7.81,2.48,9.38,6a6.11,6.11,0,0,1-2.87,7.77c-7,2.9-16.56-12.35-31.27-12-20-.48-35.69,21.15-32,40.23,5.62,28.35,40.46,33.94,54.54,8.53,12.15-14.33,22.24-1.49,15.74,12.68-22.8,47.36,48.75,61,54.64,13.42,1-15.67-9.76-20.4-19.78-29.21-6.8-6.11.74-13.93,7-7.72,4.68,8.29,7.13,18.41,16.41,23.21C274.67,198.28,299.17,173.51,293.9,151.74Z</t>
+  </si>
+  <si>
+    <t>failure_logo</t>
+  </si>
+  <si>
+    <t>M366.49,213.44c5.87-12.32-.7-24.83-7.27-35.33-16-25.82-31-53.38-48-78.68a15.82,15.82,0,0,0-24.09,1.81c-6,7.61-6.35,18.81-5.43,28a170.37,170.37,0,0,1-12.35-23.22c-7-15.37-9.36-40.45-30.87-40.81-9.36.82-14.38,8.52-13.54,17.53.85,9.22,6.59,17,9.65,25.6q10.06,22.7,22,44.5c6.17,10,9.72,22.24,19.49,29.38,13.81,9.07,27-2.08,26.33-17.24.3-.54.45-14.1,1.85-11.89,11.88,22.4,20.3,48.83,39.3,66.23C351.47,225,362.84,222.7,366.49,213.44Z</t>
+  </si>
+  <si>
+    <t>introextra_logo</t>
+  </si>
+  <si>
+    <t>M348.9,323.2c-3.47-16.11-11.47-30.3-29.86-21.27-19.57,12.55,0,54.13-29.41,56.46-19.94-4.59-23.08-33.33-27.77-50.2-2.95-13.1-6.15-26.45-13.34-37.79-13.79-24.19-46.38-28.09-62.93-4.68-13.1,16.86-26.18,67.82,7,68.52,22.21-5,11-33.13,23.18-34.69,5.21.16,6.61,6.3,6.73,10.59,1.49,18.9,4.3,38.06,12.6,55.11C268.41,437.45,365,395.85,348.9,323.2Z</t>
+  </si>
+  <si>
+    <t>interest_logo</t>
+  </si>
+  <si>
+    <t>senses_logo</t>
+  </si>
+  <si>
+    <t>M361.11,153.38a14,14,0,0,1,9.65,4.57c4.29,5,3.9,12.69.84,18.5s-8.25,10.12-13.32,14.28L326.91,216.5c-2.59,2.13-5.25,4.34-6.83,7.3s-1.83,6.89.3,9.48,6,3.1,9.17,2.23,6-2.9,8.71-4.77a128.53,128.53,0,0,1,43.13-18.89c6-1.4,12.35-2.35,18.31-.72s11.42,6.4,12.1,12.54c.58,5.15-2.31,10.22-6.31,13.51s-9,5.08-14,6.58A169,169,0,0,1,342.84,251c-4,0-8.24-.11-12,1.51s-6.77,5.56-5.9,9.52c.66,3,3.46,5.25,6.44,6.12s6.17.67,9.27.45l42.59-3c8.44-.6,17.23-1.14,25.07,2.05s14.35,11.34,12.75,19.65c-1.46,7.6-9.19,12.7-16.87,13.66s-15.35-1.31-22.76-3.56L343,285.67c-3-.92-6.18-1.85-9.33-1.46s-6.31,2.49-6.91,5.6c-1,5.19,4.93,8.76,9.86,10.65l45.16,17.39c5.69,2.19,11.53,4.48,15.93,8.7s7,10.9,4.71,16.54-8.55,8.49-14.49,8.47-11.58-2.45-16.9-5.11c-16.28-8.13-31.25-18.64-46-29.28-12.1-8.71-24.33-17.76-32.9-29.95-6.34-9-10.35-20-10-31.07s2.47-17.74,8.36-27.32a422.12,422.12,0,0,1,45.88-61.35c4.54-5,9.4-10.11,15.67-12.68A19.88,19.88,0,0,1,361.11,153.38Z</t>
+  </si>
+  <si>
+    <t>element_logo</t>
+  </si>
+  <si>
+    <t>M83.14,199.1c-9.1,7.76-13.77,19.14-20.56,28.82a78.51,78.51,0,0,1-42.74,30.24c-2.52.7-5.76,2.44-4.91,4.91.71,2,3.52,2.09,5.66,1.83,54.25-9.74,83.64,39.76,120,10.84C190,235.71,135.09,159.38,83.14,199.1Z</t>
+  </si>
+  <si>
+    <t>direction_logo</t>
+  </si>
+  <si>
+    <t>M301.13,263.45c8.11-20.46-49.55-20-61.88-23.46-11.1-.11-14.8-11.34-23.5-16-18-9.54-24.81,2.63-33.71.38-4.14-3.24-3.92-9.6-7.12-13.71a27.68,27.68,0,0,0-26.48-12.92c-9.2,1-39.33,10.89-34.18,23.29,1.48,3.31,5,5.4,8.61,5.85,4.17.52,7.89-.94,11.62-2.57,31.62-13.67,15.07,17.56,44.74,21.54,3.78.58,8,.78,11.55-.44,15.63-4.59,17.25,16.78,44.2,20.45,9.12,2.15,18.49,3,27.82,3.83C273.92,270.53,295.26,275.8,301.13,263.45Z</t>
+  </si>
+  <si>
+    <t>success_logo</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Le cadre du portrait</t>
+  </si>
+  <si>
+    <t>frame</t>
+  </si>
+  <si>
+    <t>frame_logo</t>
+  </si>
+  <si>
+    <t>#d9ac4f</t>
+  </si>
+  <si>
+    <t>M391.05,250.09c0,24.8.08,49.6,0,74.39a171.61,171.61,0,0,1-26.39,91.81c-17,27.22-40.05,47.79-68.42,62.52a181.22,181.22,0,0,1-52.07,17.48,186.62,186.62,0,0,1-41,2.74c-37.22-1.64-71.15-13-101.37-34.95a168.54,168.54,0,0,1-43.33-45.75A172.22,172.22,0,0,1,30.89,325.2q0-75.46,0-150.92A168.88,168.88,0,0,1,48,100.54,173.94,173.94,0,0,1,60.34,79.11C77.09,54,99.21,35,125.91,21.19A182.33,182.33,0,0,1,176.84,4a188.56,188.56,0,0,1,43-2.81,183.65,183.65,0,0,1,76.51,20.22,176,176,0,0,1,43.35,31.35,163,163,0,0,1,20.35,24.07,174,174,0,0,1,26.25,58.7,176,176,0,0,1,4.2,27.12c.31,4.15.49,8.32.5,12.49Q391.09,212.61,391.05,250.09Z</t>
   </si>
   <si>
     <t>Athlete</t>
@@ -1195,11 +1290,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -1241,7 +1336,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1275,21 +1370,20 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1518,6 +1612,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="14.88"/>
     <col customWidth="1" min="5" max="5" width="31.75"/>
     <col customWidth="1" min="6" max="6" width="20.75"/>
     <col customWidth="1" min="7" max="7" width="27.13"/>
@@ -1738,8 +1833,8 @@
       <c r="J5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>35</v>
+      <c r="K5" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>35</v>
@@ -1794,8 +1889,8 @@
       <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>35</v>
+      <c r="K6" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>35</v>
@@ -1906,8 +2001,8 @@
       <c r="J8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>35</v>
+      <c r="K8" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>35</v>
@@ -2118,8 +2213,8 @@
       <c r="J12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="4" t="s">
-        <v>35</v>
+      <c r="K12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>35</v>
@@ -2330,8 +2425,8 @@
       <c r="J16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>35</v>
+      <c r="K16" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>35</v>
@@ -2533,8 +2628,8 @@
       <c r="J20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K20" s="4" t="s">
-        <v>35</v>
+      <c r="K20" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>35</v>
@@ -2952,8 +3047,8 @@
       <c r="J29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K29" s="4" t="s">
-        <v>35</v>
+      <c r="K29" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>35</v>
@@ -3110,8 +3205,8 @@
       <c r="J32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K32" s="4" t="s">
-        <v>35</v>
+      <c r="K32" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>35</v>
@@ -3261,8 +3356,8 @@
       <c r="J35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>35</v>
+      <c r="K35" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>35</v>
@@ -3473,8 +3568,8 @@
       <c r="J39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K39" s="4" t="s">
-        <v>35</v>
+      <c r="K39" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>35</v>
@@ -3720,8 +3815,8 @@
       <c r="J44" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K44" s="4" t="s">
-        <v>35</v>
+      <c r="K44" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>35</v>
@@ -4112,19 +4207,648 @@
         <v>239</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M52" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
     <row r="53">
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="K53" s="14"/>
-      <c r="O53" s="15"/>
+      <c r="A53" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q53" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P55" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q55" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P56" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q56" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P57" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q57" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>14.0</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L58" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M58" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>15.0</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L59" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M59" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N59" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q59" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2">
+        <v>16.0</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N60" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>17.0</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N61" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P61" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q61" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>19.0</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P62" s="6"/>
+      <c r="Q62" s="6"/>
+      <c r="R62" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P63" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C10"/>
     <hyperlink r:id="rId2" ref="C11"/>
     <hyperlink r:id="rId3" ref="C12"/>
+    <hyperlink r:id="rId4" ref="C55"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -4143,19 +4867,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>32</v>
@@ -4198,26 +4922,26 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="s">
-        <v>245</v>
+      <c r="A2" s="13" t="s">
+        <v>272</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>251</v>
+        <v>276</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>278</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>54</v>
@@ -4225,11 +4949,11 @@
       <c r="I2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>252</v>
+      <c r="J2" s="16" t="s">
+        <v>279</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>92</v>
@@ -4237,8 +4961,8 @@
       <c r="M2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="19" t="s">
-        <v>254</v>
+      <c r="N2" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>161</v>
@@ -4250,30 +4974,30 @@
         <v>190</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="15" t="s">
-        <v>256</v>
+      <c r="A3" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>261</v>
+        <v>286</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>288</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>54</v>
@@ -4281,11 +5005,11 @@
       <c r="I3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>262</v>
+      <c r="J3" s="16" t="s">
+        <v>289</v>
       </c>
       <c r="K3" s="9" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>96</v>
@@ -4293,8 +5017,8 @@
       <c r="M3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="19" t="s">
-        <v>264</v>
+      <c r="N3" s="17" t="s">
+        <v>291</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>161</v>
@@ -4306,30 +5030,30 @@
         <v>190</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="15" t="s">
-        <v>266</v>
+      <c r="A4" s="18" t="s">
+        <v>293</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>270</v>
+        <v>295</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>297</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>54</v>
@@ -4337,11 +5061,11 @@
       <c r="I4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>271</v>
+      <c r="J4" s="16" t="s">
+        <v>298</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>99</v>
@@ -4349,8 +5073,8 @@
       <c r="M4" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N4" s="19" t="s">
-        <v>273</v>
+      <c r="N4" s="17" t="s">
+        <v>300</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>161</v>
@@ -4362,30 +5086,30 @@
         <v>194</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="16" t="s">
-        <v>275</v>
+      <c r="A5" s="13" t="s">
+        <v>302</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>280</v>
+        <v>305</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>307</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>54</v>
@@ -4393,11 +5117,11 @@
       <c r="I5" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>281</v>
+      <c r="J5" s="16" t="s">
+        <v>308</v>
       </c>
       <c r="K5" s="9" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>99</v>
@@ -4405,8 +5129,8 @@
       <c r="M5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N5" s="19" t="s">
-        <v>283</v>
+      <c r="N5" s="17" t="s">
+        <v>310</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>153</v>
@@ -4418,30 +5142,30 @@
         <v>190</v>
       </c>
       <c r="R5" s="9" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="16" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>289</v>
+        <v>314</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>54</v>
@@ -4449,11 +5173,11 @@
       <c r="I6" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="14" t="s">
-        <v>290</v>
+      <c r="J6" s="16" t="s">
+        <v>317</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>291</v>
+        <v>318</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>96</v>
@@ -4461,8 +5185,8 @@
       <c r="M6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="19" t="s">
-        <v>292</v>
+      <c r="N6" s="17" t="s">
+        <v>319</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>157</v>
@@ -4474,30 +5198,30 @@
         <v>190</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
-        <v>294</v>
+      <c r="A7" s="18" t="s">
+        <v>321</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>298</v>
+        <v>323</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>54</v>
@@ -4505,11 +5229,11 @@
       <c r="I7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="14" t="s">
-        <v>299</v>
+      <c r="J7" s="16" t="s">
+        <v>326</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>96</v>
@@ -4517,8 +5241,8 @@
       <c r="M7" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N7" s="19" t="s">
-        <v>301</v>
+      <c r="N7" s="17" t="s">
+        <v>328</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>157</v>
@@ -4530,30 +5254,30 @@
         <v>190</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="s">
-        <v>303</v>
+      <c r="A8" s="13" t="s">
+        <v>330</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>306</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>307</v>
+        <v>332</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>334</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>58</v>
@@ -4561,11 +5285,11 @@
       <c r="I8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="14" t="s">
-        <v>308</v>
+      <c r="J8" s="16" t="s">
+        <v>335</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>96</v>
@@ -4573,8 +5297,8 @@
       <c r="M8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>310</v>
+      <c r="N8" s="17" t="s">
+        <v>337</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>161</v>
@@ -4586,30 +5310,30 @@
         <v>197</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="s">
-        <v>312</v>
+      <c r="A9" s="18" t="s">
+        <v>339</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>316</v>
+        <v>341</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>343</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>49</v>
@@ -4617,11 +5341,11 @@
       <c r="I9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="14" t="s">
-        <v>252</v>
+      <c r="J9" s="16" t="s">
+        <v>279</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>317</v>
+        <v>344</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>96</v>
@@ -4629,8 +5353,8 @@
       <c r="M9" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="19" t="s">
-        <v>318</v>
+      <c r="N9" s="17" t="s">
+        <v>345</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>153</v>
@@ -4642,30 +5366,30 @@
         <v>190</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>319</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="15" t="s">
-        <v>320</v>
+      <c r="A10" s="18" t="s">
+        <v>347</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>323</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>324</v>
+        <v>349</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>351</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>58</v>
@@ -4673,11 +5397,11 @@
       <c r="I10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>325</v>
+      <c r="J10" s="16" t="s">
+        <v>352</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>326</v>
+        <v>353</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>96</v>
@@ -4685,8 +5409,8 @@
       <c r="M10" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N10" s="19" t="s">
-        <v>327</v>
+      <c r="N10" s="17" t="s">
+        <v>354</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>161</v>
@@ -4698,30 +5422,30 @@
         <v>190</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>328</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="15" t="s">
-        <v>329</v>
+      <c r="A11" s="18" t="s">
+        <v>356</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>330</v>
+        <v>357</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>333</v>
+        <v>358</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>360</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>58</v>
@@ -4729,11 +5453,11 @@
       <c r="I11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="14" t="s">
-        <v>334</v>
+      <c r="J11" s="16" t="s">
+        <v>361</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>96</v>
@@ -4741,8 +5465,8 @@
       <c r="M11" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N11" s="19" t="s">
-        <v>336</v>
+      <c r="N11" s="17" t="s">
+        <v>363</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>157</v>
@@ -4754,30 +5478,30 @@
         <v>190</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>337</v>
+        <v>364</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="16" t="s">
-        <v>338</v>
+      <c r="A12" s="13" t="s">
+        <v>365</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>339</v>
+        <v>366</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>341</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>342</v>
+        <v>367</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>368</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>369</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>58</v>
@@ -4785,11 +5509,11 @@
       <c r="I12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>252</v>
+      <c r="J12" s="16" t="s">
+        <v>279</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>343</v>
+        <v>370</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>99</v>
@@ -4797,8 +5521,8 @@
       <c r="M12" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="19" t="s">
-        <v>344</v>
+      <c r="N12" s="17" t="s">
+        <v>371</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>157</v>
@@ -4810,30 +5534,30 @@
         <v>190</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>345</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="15" t="s">
-        <v>346</v>
+      <c r="A13" s="18" t="s">
+        <v>373</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>347</v>
+        <v>374</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>349</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>350</v>
+        <v>375</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>377</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>49</v>
@@ -4841,11 +5565,11 @@
       <c r="I13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="14" t="s">
-        <v>351</v>
+      <c r="J13" s="16" t="s">
+        <v>378</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>352</v>
+        <v>379</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>92</v>
@@ -4853,8 +5577,8 @@
       <c r="M13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="N13" s="19" t="s">
-        <v>353</v>
+      <c r="N13" s="17" t="s">
+        <v>380</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>161</v>
@@ -4866,30 +5590,30 @@
         <v>194</v>
       </c>
       <c r="R13" s="9" t="s">
-        <v>354</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="s">
-        <v>355</v>
+      <c r="A14" s="13" t="s">
+        <v>382</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>356</v>
+        <v>383</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>359</v>
+        <v>384</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>386</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>58</v>
@@ -4897,11 +5621,11 @@
       <c r="I14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>360</v>
+      <c r="J14" s="16" t="s">
+        <v>387</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>361</v>
+        <v>388</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>96</v>
@@ -4909,8 +5633,8 @@
       <c r="M14" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N14" s="19" t="s">
-        <v>362</v>
+      <c r="N14" s="17" t="s">
+        <v>389</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>157</v>
@@ -4922,152 +5646,152 @@
         <v>197</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>363</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16">
-      <c r="S16" s="15"/>
+      <c r="S16" s="18"/>
     </row>
     <row r="17">
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
     </row>
     <row r="18">
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
     </row>
     <row r="19">
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
     </row>
     <row r="20">
-      <c r="I20" s="20"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
     </row>
     <row r="21">
-      <c r="I21" s="20"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
     </row>
     <row r="22">
-      <c r="I22" s="20"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
     </row>
     <row r="23">
-      <c r="I23" s="20"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
     </row>
     <row r="24">
-      <c r="I24" s="20"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
     <row r="25">
-      <c r="I25" s="20"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
     </row>
     <row r="26">
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
     </row>
     <row r="27">
-      <c r="I27" s="20"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
     </row>
     <row r="28">
-      <c r="I28" s="20"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>